<commit_message>
Derived Stat Gameplay Effect added. Created Stat Calculator
</commit_message>
<xml_diff>
--- a/AuraSecondaryAttributes.xlsx
+++ b/AuraSecondaryAttributes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d642cadae599aab/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\GAS\Aura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{292D5397-6139-4E20-9F82-2C7570A15CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD20D403-C4EB-47B7-82E8-8767768A5E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{A1629ED0-9F43-4B05-953D-F59051BD8AAA}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Str</t>
   </si>
@@ -59,15 +60,9 @@
     <t>Increase Health</t>
   </si>
   <si>
-    <t>Primary</t>
-  </si>
-  <si>
     <t>Effect</t>
   </si>
   <si>
-    <t>Secondary</t>
-  </si>
-  <si>
     <t>Armor</t>
   </si>
   <si>
@@ -77,9 +72,6 @@
     <t>Armor Penetration</t>
   </si>
   <si>
-    <t>Add. Secondary</t>
-  </si>
-  <si>
     <t>Block Chance</t>
   </si>
   <si>
@@ -132,13 +124,43 @@
   </si>
   <si>
     <t>Health Regeneration</t>
+  </si>
+  <si>
+    <t>Base Value</t>
+  </si>
+  <si>
+    <t>Primary Stats</t>
+  </si>
+  <si>
+    <t>Derived Primary</t>
+  </si>
+  <si>
+    <t>Secondary Stats</t>
+  </si>
+  <si>
+    <t>Derived Stats by Primary Stats</t>
+  </si>
+  <si>
+    <t>Derived Stats by Secondary Stats</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Pre Multiply</t>
+  </si>
+  <si>
+    <t>Post Multiply</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,16 +168,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -163,12 +205,298 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,188 +831,505 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6AC6BB-FE8C-4431-A9A6-C99ECC6BFF59}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="4" width="34.81640625" customWidth="1"/>
+    <col min="5" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" customWidth="1"/>
+    <col min="9" max="9" width="51.1796875" customWidth="1"/>
+    <col min="10" max="10" width="7.6328125" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" customWidth="1"/>
+    <col min="12" max="12" width="16.6328125" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="19.453125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="53.7265625" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.7265625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="10"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="14"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="16"/>
+      <c r="C5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="16"/>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="16"/>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="16"/>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>17</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="16"/>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>12</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="16"/>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E10" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="16"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="16"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="16"/>
+      <c r="C13" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="16"/>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="16"/>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2">
+        <f t="shared" ref="H15:H20" si="0">(VLOOKUP(C15,$C$6:$G$10,2,FALSE)+F15)*E15+G15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="16"/>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="16"/>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B18" s="16"/>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B19" s="16"/>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="16"/>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="16"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B22" s="16"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B23" s="16"/>
+      <c r="C23" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B24" s="16"/>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B25" s="16"/>
+      <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2">
+        <f>(VLOOKUP(C25,$D$14:$I$20,5,FALSE)+F25)*E25+G25</f>
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="I25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B26" s="16"/>
+      <c r="C26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2">
+        <f>(VLOOKUP(C26,$D$14:$I$20,5,FALSE)+F18)*E26+G26</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="16"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B27" s="16"/>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2">
+        <f>(VLOOKUP(C27,$D$14:$I$20,5,FALSE)+F19)*E27+G27</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B28" s="16"/>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2">
+        <f>(VLOOKUP(C28,$D$14:$I$20,5,FALSE)+F20)*E28+G28</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-    </row>
+      <c r="J28" s="17"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B29" s="14"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B30" s="9"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>